<commit_message>
tutorial 2 -ok / tutorial 3 -ing
</commit_message>
<xml_diff>
--- a/MyApplication_2/TouchGFX/assets/texts/texts.xlsx
+++ b/MyApplication_2/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="66">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -161,15 +161,15 @@
     <t xml:space="preserve">SingleUseId2</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Left</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;value&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId3</t>
-  </si>
-  <si>
     <t xml:space="preserve">00</t>
   </si>
   <si>
@@ -200,10 +200,19 @@
     <t xml:space="preserve">SingleUseId9</t>
   </si>
   <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
     <t xml:space="preserve">SingleUseId10</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;hour&gt;:&lt;min&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1492,9 @@
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -1714,18 +1725,18 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
@@ -1753,10 +1764,10 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
@@ -1765,29 +1776,29 @@
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
         <v>56</v>
@@ -1804,10 +1815,10 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -1816,23 +1827,74 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>44</v>
       </c>
       <c r="F12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>